<commit_message>
working code after testing the agent_analyzer
</commit_message>
<xml_diff>
--- a/workspace/input/test_cases_template.xlsx
+++ b/workspace/input/test_cases_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29728"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_D99D7BC48D9ECF122363E8815C05B45C88711109" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6DF1E16-29A9-4975-BC87-0339BA6B8F3C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8D77F14-57BB-4A06-8EDE-FA8C70CBFE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="173">
   <si>
     <t>TC_ID</t>
   </si>
@@ -89,30 +89,33 @@
     <t>Launch</t>
   </si>
   <si>
+    <t>https://dev.erosnow.com</t>
+  </si>
+  <si>
+    <t>Verify website launches</t>
+  </si>
+  <si>
+    <t>Open www.dev.erosnow.com</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Browser is open</t>
+  </si>
+  <si>
+    <t>Launch website</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
     <t>www.dev.erosnow.com</t>
   </si>
   <si>
-    <t>Verify website launches</t>
-  </si>
-  <si>
-    <t>Open www.dev.erosnow.com</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>Functional</t>
-  </si>
-  <si>
-    <t>Browser is open</t>
-  </si>
-  <si>
-    <t>Launch website</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t>Login</t>
   </si>
   <si>
+    <t>https://dev.erosnow.com/</t>
+  </si>
+  <si>
     <t>Login with valid credentials</t>
   </si>
   <si>
@@ -203,7 +209,7 @@
     <t>This test case validates that a logged‑in user can successfully log out of the application. The test ensures that when the user hovers over the profile icon, the dropdown menu appears containing the logout option. After clicking the logout button, the session should end, and the user should be redirected to the login page or any defined post‑logout screen, confirming that the user has been successfully logged out.</t>
   </si>
   <si>
-    <t>Browser is login</t>
+    <t>user is login</t>
   </si>
   <si>
     <t>Hover on the profile icon</t>
@@ -225,6 +231,60 @@
   </si>
   <si>
     <t>User logged out</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>Content Detail</t>
+  </si>
+  <si>
+    <t>https://dev.erosnow.com/, https://dev.erosnow.com/movie/watch/1005004/goliyon-ki-raasleela-ram-leela</t>
+  </si>
+  <si>
+    <t>Content title visible</t>
+  </si>
+  <si>
+    <t>Open content</t>
+  </si>
+  <si>
+    <t>critical</t>
+  </si>
+  <si>
+    <t>website launches and user is login</t>
+  </si>
+  <si>
+    <t>Scroll to the "Blockbuster Movies" rails</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>text='Blockbuster Movies'</t>
+  </si>
+  <si>
+    <t>Blockbuster Movies should be visible</t>
+  </si>
+  <si>
+    <t>press enter on the "goliyon ki raasleela ram leela"</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>img = 'goliyon ki raasleela ram leela'</t>
+  </si>
+  <si>
+    <t>"goliyon ki raasleela ram leela"  should be visisble</t>
+  </si>
+  <si>
+    <t>check the title on the detail page which is "goliyon ki raasleela ram leela"</t>
+  </si>
+  <si>
+    <t>text='goliyon ki raasleela ram leela'</t>
+  </si>
+  <si>
+    <t>"goliyon ki raasleela ram leela " text shoudl be visible on the detail page</t>
   </si>
   <si>
     <t>Setting</t>
@@ -498,7 +558,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,6 +604,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -593,7 +659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -620,6 +686,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -923,11 +991,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1034,70 +1102,70 @@
         <v>25</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1110,28 +1178,28 @@
         <v>2</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M4" s="3">
         <v>9284841447</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1144,26 +1212,26 @@
         <v>3</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16" ht="24">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1176,28 +1244,28 @@
         <v>4</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M6" s="13">
         <v>123456789</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16" ht="16.5">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1210,70 +1278,70 @@
         <v>5</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16" ht="99">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1286,26 +1354,113 @@
         <v>2</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" ht="16.5">
+      <c r="A10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N12" t="s">
+        <v>83</v>
+      </c>
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" error="Please select a valid priority" sqref="F2:F493" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" error="Please select a valid priority" sqref="F2:F9 F11:F493" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"P0-Blocker,P1-Critical,P2-Major,P3-Minor"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="G2:G493" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -1323,6 +1478,7 @@
     <hyperlink ref="L2" r:id="rId2" xr:uid="{4A9EFDFE-987E-4ACB-8C51-6C01CD3A75BA}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{809D97F5-02CB-48AF-B141-5DBB1FA65977}"/>
     <hyperlink ref="C8" r:id="rId4" xr:uid="{F421B40F-7579-41D1-91DE-B2285AB08B8F}"/>
+    <hyperlink ref="C10" r:id="rId5" xr:uid="{BAEB9202-F572-4420-A754-8B1499EF930E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1343,174 +1499,174 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1533,7 +1689,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8"/>
@@ -1545,13 +1701,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1559,10 +1715,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1570,10 +1726,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1581,10 +1737,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1592,10 +1748,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1603,10 +1759,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1614,10 +1770,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1625,10 +1781,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1636,10 +1792,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1647,10 +1803,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1658,10 +1814,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1669,10 +1825,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1680,80 +1836,80 @@
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1761,10 +1917,10 @@
         <v>12</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1772,10 +1928,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1783,10 +1939,10 @@
         <v>14</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1794,10 +1950,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1807,7 +1963,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="7" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -1819,35 +1975,35 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="7" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="7" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="7" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="7" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="7" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
@@ -1859,14 +2015,14 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="7" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="7" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>

</xml_diff>